<commit_message>
D0 and D1 pin setting fixed
</commit_message>
<xml_diff>
--- a/r01lib_pin_table 2.xlsx
+++ b/r01lib_pin_table 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedd/Desktop/dl/r01/r01lib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedd/dev/mcuxpresso/r01lib_FRDM_MCXC444_porting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64EA2B5-C981-914D-9959-4D84C3E68B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FE6DA8-CF95-6A47-82AA-F3C9F29C744E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30780" yWindow="900" windowWidth="41340" windowHeight="33480" activeTab="4" xr2:uid="{F4A4BD97-1D13-3141-8799-357F4902D58A}"/>
   </bookViews>
@@ -1658,7 +1658,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1704,9 +1704,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1734,6 +1731,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1748,6 +1748,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2105,20 +2108,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="14" customHeight="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="15">
       <c r="A5" s="2" t="s">
@@ -2380,7 +2383,7 @@
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="21" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2406,7 +2409,7 @@
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="24"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="3" t="s">
@@ -2430,7 +2433,7 @@
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="24"/>
+      <c r="J18" s="23"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="3" t="s">
@@ -2454,7 +2457,7 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="23"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="3" t="s">
@@ -2474,7 +2477,7 @@
       <c r="G20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="21" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="4"/>
@@ -2498,7 +2501,7 @@
       <c r="G21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="23"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
@@ -2785,7 +2788,7 @@
         <v>12</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J36" s="4"/>
@@ -2809,7 +2812,7 @@
         <v>12</v>
       </c>
       <c r="H37" s="4"/>
-      <c r="I37" s="23"/>
+      <c r="I37" s="22"/>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:14">
@@ -2876,46 +2879,46 @@
       <c r="A45" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
     </row>
     <row r="46" spans="1:14">
-      <c r="C46" s="15">
+      <c r="C46" s="24">
         <v>0</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15">
+      <c r="D46" s="24"/>
+      <c r="E46" s="24">
         <v>1</v>
       </c>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15">
+      <c r="F46" s="24"/>
+      <c r="G46" s="24">
         <v>2</v>
       </c>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15">
+      <c r="H46" s="24"/>
+      <c r="I46" s="24">
         <v>3</v>
       </c>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15">
+      <c r="J46" s="24"/>
+      <c r="K46" s="24">
         <v>4</v>
       </c>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15">
+      <c r="L46" s="24"/>
+      <c r="M46" s="24">
         <v>5</v>
       </c>
-      <c r="N46" s="15"/>
+      <c r="N46" s="24"/>
     </row>
     <row r="47" spans="1:14">
       <c r="C47" s="3" t="s">
@@ -2956,7 +2959,7 @@
       </c>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="24" t="s">
         <v>175</v>
       </c>
       <c r="B48" s="3">
@@ -3000,7 +3003,7 @@
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="15"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="3">
         <f>B48+1</f>
         <v>1</v>
@@ -3043,7 +3046,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="15"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="3">
         <f t="shared" ref="B50:B79" si="0">B49+1</f>
         <v>2</v>
@@ -3086,7 +3089,7 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="15"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3129,7 +3132,7 @@
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="15"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3172,7 +3175,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="15"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3215,7 +3218,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="15"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3258,7 +3261,7 @@
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="15"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3301,7 +3304,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="15"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3340,7 +3343,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="15"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3379,7 +3382,7 @@
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="15"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3414,7 +3417,7 @@
       <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="15"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3449,7 +3452,7 @@
       <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="15"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3484,7 +3487,7 @@
       <c r="N60" s="9"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="15"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3519,7 +3522,7 @@
       <c r="N61" s="9"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="15"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3554,7 +3557,7 @@
       <c r="N62" s="9"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="15"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3589,7 +3592,7 @@
       <c r="N63" s="9"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="15"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3624,7 +3627,7 @@
       <c r="N64" s="9"/>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="15"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3659,7 +3662,7 @@
       <c r="N65" s="9"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="15"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3694,7 +3697,7 @@
       <c r="N66" s="9"/>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="15"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3729,7 +3732,7 @@
       <c r="N67" s="9"/>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="15"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3764,7 +3767,7 @@
       <c r="N68" s="9"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="15"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3799,7 +3802,7 @@
       <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="15"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3834,7 +3837,7 @@
       <c r="N70" s="9"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="15"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3869,7 +3872,7 @@
       <c r="N71" s="9"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="15"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3892,7 +3895,7 @@
       <c r="N72" s="9"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="15"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3915,7 +3918,7 @@
       <c r="N73" s="9"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="15"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3938,7 +3941,7 @@
       <c r="N74" s="9"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="15"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3961,7 +3964,7 @@
       <c r="N75" s="9"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="15"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3984,7 +3987,7 @@
       <c r="N76" s="9"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="15"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4007,7 +4010,7 @@
       <c r="N77" s="9"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="15"/>
+      <c r="A78" s="24"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4034,7 +4037,7 @@
       <c r="N78" s="9"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="15"/>
+      <c r="A79" s="24"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4062,11 +4065,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="I36:I37"/>
     <mergeCell ref="A48:A79"/>
     <mergeCell ref="C45:N45"/>
     <mergeCell ref="C46:D46"/>
@@ -4075,6 +4073,11 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="M46:N46"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="I36:I37"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4364,7 +4367,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4389,7 +4392,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
@@ -4412,7 +4415,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
@@ -4435,7 +4438,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
@@ -4457,7 +4460,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="3"/>
@@ -4480,7 +4483,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -4578,7 +4581,7 @@
       <c r="F26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H26" s="3"/>
@@ -4601,7 +4604,7 @@
       <c r="F27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="15"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
@@ -4818,7 +4821,7 @@
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H38" s="3"/>
@@ -4839,7 +4842,7 @@
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
@@ -4904,46 +4907,46 @@
       <c r="A46" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
     </row>
     <row r="47" spans="1:14">
-      <c r="C47" s="15">
+      <c r="C47" s="24">
         <v>0</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15">
+      <c r="D47" s="24"/>
+      <c r="E47" s="24">
         <v>1</v>
       </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15">
+      <c r="F47" s="24"/>
+      <c r="G47" s="24">
         <v>2</v>
       </c>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15">
+      <c r="H47" s="24"/>
+      <c r="I47" s="24">
         <v>3</v>
       </c>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15">
+      <c r="J47" s="24"/>
+      <c r="K47" s="24">
         <v>4</v>
       </c>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15">
+      <c r="L47" s="24"/>
+      <c r="M47" s="24">
         <v>5</v>
       </c>
-      <c r="N47" s="15"/>
+      <c r="N47" s="24"/>
     </row>
     <row r="48" spans="1:14">
       <c r="C48" s="3" t="s">
@@ -4984,7 +4987,7 @@
       </c>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="24" t="s">
         <v>175</v>
       </c>
       <c r="B49" s="3">
@@ -5028,7 +5031,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="15"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="3">
         <f>B49+1</f>
         <v>1</v>
@@ -5071,7 +5074,7 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="15"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="3">
         <f t="shared" ref="B51:B80" si="0">B50+1</f>
         <v>2</v>
@@ -5114,7 +5117,7 @@
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="15"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5153,7 +5156,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="15"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5192,7 +5195,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="15"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5231,7 +5234,7 @@
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="15"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5274,7 +5277,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="15"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5317,7 +5320,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="15"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5348,7 +5351,7 @@
       <c r="N57" s="9"/>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="15"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5379,7 +5382,7 @@
       <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="15"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5410,7 +5413,7 @@
       <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="15"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5441,7 +5444,7 @@
       <c r="N60" s="9"/>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="15"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5472,7 +5475,7 @@
       <c r="N61" s="9"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="15"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5503,7 +5506,7 @@
       <c r="N62" s="9"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="15"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5538,7 +5541,7 @@
       <c r="N63" s="9"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="15"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5573,7 +5576,7 @@
       <c r="N64" s="9"/>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="15"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5608,7 +5611,7 @@
       <c r="N65" s="9"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="15"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5643,7 +5646,7 @@
       <c r="N66" s="9"/>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="15"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5678,7 +5681,7 @@
       <c r="N67" s="9"/>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="15"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5709,7 +5712,7 @@
       <c r="N68" s="9"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="15"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5740,7 +5743,7 @@
       <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="15"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5771,7 +5774,7 @@
       <c r="N70" s="9"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="15"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5802,7 +5805,7 @@
       <c r="N71" s="9"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="15"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5833,7 +5836,7 @@
       <c r="N72" s="9"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="15"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5856,7 +5859,7 @@
       <c r="N73" s="9"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="15"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5879,7 +5882,7 @@
       <c r="N74" s="9"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="15"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5902,7 +5905,7 @@
       <c r="N75" s="9"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="15"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -5925,7 +5928,7 @@
       <c r="N76" s="9"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="15"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -5948,7 +5951,7 @@
       <c r="N77" s="9"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="15"/>
+      <c r="A78" s="24"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -5971,7 +5974,7 @@
       <c r="N78" s="9"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="15"/>
+      <c r="A79" s="24"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5994,7 +5997,7 @@
       <c r="N79" s="9"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="15"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -6018,12 +6021,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I16:I19"/>
     <mergeCell ref="A49:A80"/>
     <mergeCell ref="C46:N46"/>
     <mergeCell ref="C47:D47"/>
@@ -6032,6 +6029,12 @@
     <mergeCell ref="I47:J47"/>
     <mergeCell ref="K47:L47"/>
     <mergeCell ref="M47:N47"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="I16:I19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6335,7 +6338,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="21" t="s">
         <v>27</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -6359,7 +6362,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="24"/>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="3"/>
@@ -6378,7 +6381,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="23"/>
       <c r="J19" s="1" t="s">
         <v>323</v>
       </c>
@@ -6402,7 +6405,7 @@
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="24"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="3" t="s">
@@ -6423,7 +6426,7 @@
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="23"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="3" t="s">
@@ -6444,10 +6447,10 @@
       <c r="F22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I22" s="3"/>
@@ -6471,8 +6474,8 @@
       <c r="F23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:10">
@@ -6648,7 +6651,7 @@
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6673,7 +6676,7 @@
         <v>48</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="15"/>
+      <c r="I33" s="24"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
@@ -6694,7 +6697,7 @@
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="15"/>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
@@ -6717,7 +6720,7 @@
         <v>51</v>
       </c>
       <c r="H35" s="3"/>
-      <c r="I35" s="15"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="3" t="s">
@@ -6810,7 +6813,7 @@
       <c r="F40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H40" s="3"/>
@@ -6831,7 +6834,7 @@
       <c r="F41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="15"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
@@ -6877,40 +6880,40 @@
       <c r="A47" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="C48" s="15">
+      <c r="C48" s="24">
         <v>0</v>
       </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15">
+      <c r="D48" s="24"/>
+      <c r="E48" s="24">
         <v>1</v>
       </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15">
+      <c r="F48" s="24"/>
+      <c r="G48" s="24">
         <v>2</v>
       </c>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15">
+      <c r="H48" s="24"/>
+      <c r="I48" s="24">
         <v>3</v>
       </c>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15">
+      <c r="J48" s="24"/>
+      <c r="K48" s="24">
         <v>4</v>
       </c>
-      <c r="L48" s="15"/>
+      <c r="L48" s="24"/>
     </row>
     <row r="49" spans="1:12">
       <c r="C49" s="3" t="s">
@@ -6945,7 +6948,7 @@
       </c>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="24" t="s">
         <v>175</v>
       </c>
       <c r="B50" s="3">
@@ -6979,7 +6982,7 @@
       <c r="L50" s="9"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="15"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="3">
         <f>B50+1</f>
         <v>1</v>
@@ -7012,7 +7015,7 @@
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="15"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3">
         <f t="shared" ref="B52:B81" si="0">B51+1</f>
         <v>2</v>
@@ -7045,7 +7048,7 @@
       </c>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="15"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -7078,7 +7081,7 @@
       </c>
     </row>
     <row r="54" spans="1:12">
-      <c r="A54" s="15"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7107,7 +7110,7 @@
       </c>
     </row>
     <row r="55" spans="1:12">
-      <c r="A55" s="15"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7136,7 +7139,7 @@
       </c>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="15"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7173,7 +7176,7 @@
       </c>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="15"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7206,7 +7209,7 @@
       </c>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="15"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7231,7 +7234,7 @@
       <c r="L58" s="9"/>
     </row>
     <row r="59" spans="1:12">
-      <c r="A59" s="15"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7256,7 +7259,7 @@
       <c r="L59" s="9"/>
     </row>
     <row r="60" spans="1:12">
-      <c r="A60" s="15"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7285,7 +7288,7 @@
       <c r="L60" s="9"/>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="15"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7314,7 +7317,7 @@
       <c r="L61" s="9"/>
     </row>
     <row r="62" spans="1:12">
-      <c r="A62" s="15"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7343,7 +7346,7 @@
       <c r="L62" s="9"/>
     </row>
     <row r="63" spans="1:12">
-      <c r="A63" s="15"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7372,7 +7375,7 @@
       <c r="L63" s="9"/>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="15"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7401,7 +7404,7 @@
       <c r="L64" s="9"/>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="15"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7430,7 +7433,7 @@
       <c r="L65" s="9"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="15"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7459,7 +7462,7 @@
       <c r="L66" s="9"/>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="15"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7484,7 +7487,7 @@
       <c r="L67" s="9"/>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="15"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7509,7 +7512,7 @@
       <c r="L68" s="9"/>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="15"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7538,7 +7541,7 @@
       <c r="L69" s="9"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="15"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7567,7 +7570,7 @@
       <c r="L70" s="9"/>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="15"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7596,7 +7599,7 @@
       <c r="L71" s="9"/>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="15"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7621,7 +7624,7 @@
       <c r="L72" s="9"/>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="15"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7646,7 +7649,7 @@
       <c r="L73" s="9"/>
     </row>
     <row r="74" spans="1:12">
-      <c r="A74" s="15"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7663,7 +7666,7 @@
       <c r="L74" s="9"/>
     </row>
     <row r="75" spans="1:12">
-      <c r="A75" s="15"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7680,7 +7683,7 @@
       <c r="L75" s="9"/>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="15"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -7697,7 +7700,7 @@
       <c r="L76" s="9"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="15"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -7718,7 +7721,7 @@
       <c r="L77" s="9"/>
     </row>
     <row r="78" spans="1:12">
-      <c r="A78" s="15"/>
+      <c r="A78" s="24"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -7739,7 +7742,7 @@
       <c r="L78" s="9"/>
     </row>
     <row r="79" spans="1:12">
-      <c r="A79" s="15"/>
+      <c r="A79" s="24"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -7764,7 +7767,7 @@
       <c r="L79" s="9"/>
     </row>
     <row r="80" spans="1:12">
-      <c r="A80" s="15"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -7789,7 +7792,7 @@
       <c r="L80" s="9"/>
     </row>
     <row r="81" spans="1:12">
-      <c r="A81" s="15"/>
+      <c r="A81" s="24"/>
       <c r="B81" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -7815,6 +7818,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A50:A81"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
     <mergeCell ref="G40:G41"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:I4"/>
@@ -7822,13 +7832,6 @@
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="I17:I21"/>
-    <mergeCell ref="A50:A81"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8127,7 +8130,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -8152,7 +8155,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
@@ -8175,7 +8178,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
@@ -8198,7 +8201,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
@@ -8217,10 +8220,10 @@
       <c r="F20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="3"/>
@@ -8242,8 +8245,8 @@
       <c r="F21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -8581,7 +8584,7 @@
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H38" s="3"/>
@@ -8602,7 +8605,7 @@
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
@@ -8622,7 +8625,7 @@
         <v>12</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I40" s="3"/>
@@ -8643,7 +8646,7 @@
         <v>12</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="15"/>
+      <c r="H41" s="24"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:10">
@@ -8700,22 +8703,22 @@
       <c r="J47" s="29"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="C48" s="15">
+      <c r="C48" s="24">
         <v>0</v>
       </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15">
+      <c r="D48" s="24"/>
+      <c r="E48" s="24">
         <v>1</v>
       </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15">
+      <c r="F48" s="24"/>
+      <c r="G48" s="24">
         <v>2</v>
       </c>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15">
+      <c r="H48" s="24"/>
+      <c r="I48" s="24">
         <v>3</v>
       </c>
-      <c r="J48" s="15"/>
+      <c r="J48" s="24"/>
     </row>
     <row r="49" spans="1:10">
       <c r="C49" s="3" t="s">
@@ -8744,7 +8747,7 @@
       </c>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="24" t="s">
         <v>175</v>
       </c>
       <c r="B50" s="3">
@@ -8776,7 +8779,7 @@
       </c>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="15"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="3">
         <f>B50+1</f>
         <v>1</v>
@@ -8807,7 +8810,7 @@
       </c>
     </row>
     <row r="52" spans="1:10">
-      <c r="A52" s="15"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3">
         <f t="shared" ref="B52:B81" si="0">B51+1</f>
         <v>2</v>
@@ -8834,7 +8837,7 @@
       <c r="J52" s="9"/>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="15"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8861,7 +8864,7 @@
       <c r="J53" s="9"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="15"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8884,7 +8887,7 @@
       <c r="J54" s="9"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="15"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8907,7 +8910,7 @@
       <c r="J55" s="9"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="15"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8938,7 +8941,7 @@
       </c>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="15"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8965,7 +8968,7 @@
       </c>
     </row>
     <row r="58" spans="1:10">
-      <c r="A58" s="15"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8988,7 +8991,7 @@
       </c>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="15"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -9011,7 +9014,7 @@
       </c>
     </row>
     <row r="60" spans="1:10">
-      <c r="A60" s="15"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -9034,7 +9037,7 @@
       </c>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="15"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -9057,7 +9060,7 @@
       </c>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="15"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -9084,7 +9087,7 @@
       </c>
     </row>
     <row r="63" spans="1:10">
-      <c r="A63" s="15"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -9111,7 +9114,7 @@
       </c>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="15"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -9130,7 +9133,7 @@
       </c>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="15"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -9149,7 +9152,7 @@
       </c>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="15"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -9172,7 +9175,7 @@
       <c r="J66" s="9"/>
     </row>
     <row r="67" spans="1:10">
-      <c r="A67" s="15"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -9191,7 +9194,7 @@
       <c r="J67" s="9"/>
     </row>
     <row r="68" spans="1:10">
-      <c r="A68" s="15"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -9206,7 +9209,7 @@
       <c r="J68" s="9"/>
     </row>
     <row r="69" spans="1:10">
-      <c r="A69" s="15"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -9221,7 +9224,7 @@
       <c r="J69" s="9"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="A70" s="15"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -9236,7 +9239,7 @@
       <c r="J70" s="9"/>
     </row>
     <row r="71" spans="1:10">
-      <c r="A71" s="15"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -9251,7 +9254,7 @@
       <c r="J71" s="9"/>
     </row>
     <row r="72" spans="1:10">
-      <c r="A72" s="15"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -9266,7 +9269,7 @@
       <c r="J72" s="9"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="A73" s="15"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -9281,7 +9284,7 @@
       <c r="J73" s="9"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="A74" s="15"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -9296,7 +9299,7 @@
       <c r="J74" s="9"/>
     </row>
     <row r="75" spans="1:10">
-      <c r="A75" s="15"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -9311,7 +9314,7 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="A76" s="15"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -9326,7 +9329,7 @@
       <c r="J76" s="9"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="A77" s="15"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -9345,7 +9348,7 @@
       </c>
     </row>
     <row r="78" spans="1:10">
-      <c r="A78" s="15"/>
+      <c r="A78" s="24"/>
       <c r="B78" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -9364,7 +9367,7 @@
       </c>
     </row>
     <row r="79" spans="1:10">
-      <c r="A79" s="15"/>
+      <c r="A79" s="24"/>
       <c r="B79" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -9387,7 +9390,7 @@
       </c>
     </row>
     <row r="80" spans="1:10">
-      <c r="A80" s="15"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -9410,7 +9413,7 @@
       </c>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="15"/>
+      <c r="A81" s="24"/>
       <c r="B81" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -9434,6 +9437,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A50:A81"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="H40:H41"/>
     <mergeCell ref="G38:G39"/>
@@ -9441,12 +9450,6 @@
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="G20:G21"/>
     <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A50:A81"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9457,8 +9460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5A993D-0126-8C42-A678-2DEBB1B57B8D}">
   <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N97" sqref="N97:N99"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.7109375" defaultRowHeight="14"/>
@@ -9740,7 +9743,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -9765,7 +9768,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
@@ -9788,7 +9791,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
@@ -9811,7 +9814,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="15"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
@@ -9832,10 +9835,10 @@
       <c r="F20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="3"/>
@@ -9859,8 +9862,8 @@
       <c r="F21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9">
@@ -10220,7 +10223,7 @@
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H38" s="3"/>
@@ -10243,7 +10246,7 @@
       <c r="F39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
@@ -10263,7 +10266,7 @@
         <v>12</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="22" t="s">
+      <c r="H40" s="21" t="s">
         <v>27</v>
       </c>
       <c r="I40" s="3"/>
@@ -10280,7 +10283,7 @@
         <v>12</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="23"/>
+      <c r="H41" s="22"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:12">
@@ -10341,26 +10344,26 @@
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15" t="s">
+      <c r="D48" s="24"/>
+      <c r="E48" s="24" t="s">
         <v>372</v>
       </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15" t="s">
+      <c r="F48" s="24"/>
+      <c r="G48" s="24" t="s">
         <v>373</v>
       </c>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15" t="s">
+      <c r="H48" s="24"/>
+      <c r="I48" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15" t="s">
+      <c r="J48" s="24"/>
+      <c r="K48" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="L48" s="15"/>
+      <c r="L48" s="24"/>
     </row>
     <row r="49" spans="1:14">
       <c r="C49" s="3" t="s">
@@ -10395,7 +10398,7 @@
       </c>
     </row>
     <row r="50" spans="1:14">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="24" t="s">
         <v>175</v>
       </c>
       <c r="B50" s="3">
@@ -10437,16 +10440,16 @@
       </c>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="15"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="3">
         <f>B50+1</f>
         <v>1</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>170</v>
+      <c r="D51" s="30" t="s">
+        <v>171</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>361</v>
@@ -10473,21 +10476,21 @@
         <v>171</v>
       </c>
       <c r="N51" s="1" t="str">
-        <f t="shared" ref="N51:N62" si="0">C51</f>
+        <f t="shared" ref="N51:N55" si="0">C51</f>
         <v>PTA1</v>
       </c>
     </row>
     <row r="52" spans="1:14">
-      <c r="A52" s="15"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3">
         <f t="shared" ref="B52:B81" si="1">B51+1</f>
         <v>2</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>170</v>
+      <c r="D52" s="30" t="s">
+        <v>171</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>363</v>
@@ -10515,7 +10518,7 @@
       </c>
     </row>
     <row r="53" spans="1:14">
-      <c r="A53" s="15"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -10552,7 +10555,7 @@
       </c>
     </row>
     <row r="54" spans="1:14">
-      <c r="A54" s="15"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="3">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -10585,7 +10588,7 @@
       </c>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="15"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="3">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -10618,7 +10621,7 @@
       </c>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="15"/>
+      <c r="A56" s="24"/>
       <c r="B56" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -10647,7 +10650,7 @@
       </c>
     </row>
     <row r="57" spans="1:14">
-      <c r="A57" s="15"/>
+      <c r="A57" s="24"/>
       <c r="B57" s="3">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -10676,7 +10679,7 @@
       </c>
     </row>
     <row r="58" spans="1:14">
-      <c r="A58" s="15"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -10697,7 +10700,7 @@
       </c>
     </row>
     <row r="59" spans="1:14">
-      <c r="A59" s="15"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -10718,7 +10721,7 @@
       </c>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="15"/>
+      <c r="A60" s="24"/>
       <c r="B60" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -10739,7 +10742,7 @@
       </c>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="15"/>
+      <c r="A61" s="24"/>
       <c r="B61" s="3">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -10760,7 +10763,7 @@
       </c>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="15"/>
+      <c r="A62" s="24"/>
       <c r="B62" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -10780,12 +10783,12 @@
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="N62" s="1" t="str">
-        <f t="shared" ref="N62:N65" si="2">E51</f>
+        <f t="shared" ref="N62:N64" si="2">E51</f>
         <v>PTB1</v>
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="15"/>
+      <c r="A63" s="24"/>
       <c r="B63" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -10810,7 +10813,7 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="15"/>
+      <c r="A64" s="24"/>
       <c r="B64" s="3">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -10831,7 +10834,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="15"/>
+      <c r="A65" s="24"/>
       <c r="B65" s="3">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -10852,7 +10855,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="15"/>
+      <c r="A66" s="24"/>
       <c r="B66" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -10872,12 +10875,12 @@
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="N66" s="1" t="str">
-        <f t="shared" ref="N66:N71" si="3">E67</f>
+        <f t="shared" ref="N66:N68" si="3">E67</f>
         <v>PTB17</v>
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="15"/>
+      <c r="A67" s="24"/>
       <c r="B67" s="3">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -10902,7 +10905,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="15"/>
+      <c r="A68" s="24"/>
       <c r="B68" s="3">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -10931,7 +10934,7 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="15"/>
+      <c r="A69" s="24"/>
       <c r="B69" s="3">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -10960,7 +10963,7 @@
       </c>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="15"/>
+      <c r="A70" s="24"/>
       <c r="B70" s="3">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -10988,12 +10991,12 @@
         <v>171</v>
       </c>
       <c r="N70" s="1" t="str">
-        <f t="shared" ref="N70:N80" si="4">G51</f>
+        <f t="shared" ref="N70:N76" si="4">G51</f>
         <v>PTC1</v>
       </c>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="15"/>
+      <c r="A71" s="24"/>
       <c r="B71" s="3">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -11022,7 +11025,7 @@
       </c>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="15"/>
+      <c r="A72" s="24"/>
       <c r="B72" s="3">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -11051,7 +11054,7 @@
       </c>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="15"/>
+      <c r="A73" s="24"/>
       <c r="B73" s="3">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -11080,7 +11083,7 @@
       </c>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="15"/>
+      <c r="A74" s="24"/>
       <c r="B74" s="3">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -11105,7 +11108,7 @@
       </c>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="15"/>
+      <c r="A75" s="24"/>
       <c r="B75" s="3">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -11130,7 +11133,7 @@
       </c>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="15"/>
+      <c r="A76" s="24"/>
       <c r="B76" s="3">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -11151,7 +11154,7 @@
       </c>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="15"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="3">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -11172,7 +11175,7 @@
       </c>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="15"/>
+      <c r="A78" s="24"/>
       <c r="B78" s="3">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -11193,7 +11196,7 @@
       </c>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="15"/>
+      <c r="A79" s="24"/>
       <c r="B79" s="3">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -11218,7 +11221,7 @@
       </c>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="15"/>
+      <c r="A80" s="24"/>
       <c r="B80" s="3">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -11243,7 +11246,7 @@
       </c>
     </row>
     <row r="81" spans="1:14">
-      <c r="A81" s="15"/>
+      <c r="A81" s="24"/>
       <c r="B81" s="3">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -11269,7 +11272,7 @@
     </row>
     <row r="82" spans="1:14">
       <c r="N82" s="1" t="str">
-        <f t="shared" ref="N82:N89" si="6">I51</f>
+        <f t="shared" ref="N82:N88" si="6">I51</f>
         <v>PTD1</v>
       </c>
     </row>
@@ -11329,7 +11332,7 @@
     </row>
     <row r="92" spans="1:14">
       <c r="N92" s="1" t="str">
-        <f t="shared" ref="N92:N109" si="7">K71</f>
+        <f t="shared" ref="N92:N96" si="7">K71</f>
         <v>PTE21</v>
       </c>
     </row>
@@ -11377,12 +11380,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
     <mergeCell ref="A50:A81"/>
     <mergeCell ref="K48:L48"/>
     <mergeCell ref="H40:H41"/>
@@ -11391,6 +11388,12 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="G48:H48"/>
     <mergeCell ref="I48:J48"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11560,6 +11563,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="43135f08-7c27-4a7c-bc6d-152a25501e39" xsi:nil="true"/>
@@ -11568,15 +11580,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11787,20 +11790,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993051E6-CE55-49FB-9812-9A2B302725FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D7A352-4E74-4D3B-B371-7F84A478DD81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="43135f08-7c27-4a7c-bc6d-152a25501e39"/>
     <ds:schemaRef ds:uri="6946600b-d432-4ec1-a6de-e6a1f3354bfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{993051E6-CE55-49FB-9812-9A2B302725FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>